<commit_message>
Adicionando analise de custos
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3.305555555555555</v>
+        <v>5.375</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3.305555555555555</v>
+        <v>5.375</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5.944444444444445</v>
+        <v>6.875</v>
       </c>
       <c r="C4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.58333333333333</v>
+        <v>12.875</v>
       </c>
       <c r="C5" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
@@ -509,10 +509,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>23.86111111111111</v>
+        <v>34.04166666666666</v>
       </c>
       <c r="C6" t="n">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
@@ -522,10 +522,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4.777777777777778</v>
+        <v>6.875</v>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionando grafico de fluxo de caixa
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.375</v>
+        <v>5.041666666666667</v>
       </c>
       <c r="C2" t="n">
         <v>6</v>
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5.375</v>
+        <v>5.041666666666667</v>
       </c>
       <c r="C3" t="n">
         <v>6</v>
@@ -483,10 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.875</v>
+        <v>3.875</v>
       </c>
       <c r="C4" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12.875</v>
+        <v>8.208333333333334</v>
       </c>
       <c r="C5" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
@@ -509,10 +509,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>34.04166666666666</v>
+        <v>18.625</v>
       </c>
       <c r="C6" t="n">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7">
@@ -522,10 +522,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>6.875</v>
+        <v>3.458333333333333</v>
       </c>
       <c r="C7" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionando simulação de monte carlo
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.041666666666667</v>
+        <v>4.916666666666667</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5.041666666666667</v>
+        <v>4.916666666666667</v>
       </c>
       <c r="C3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3.875</v>
+        <v>3.958333333333333</v>
       </c>
       <c r="C4" t="n">
         <v>4</v>
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8.208333333333334</v>
+        <v>8.041666666666666</v>
       </c>
       <c r="C5" t="n">
         <v>9</v>
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>18.625</v>
+        <v>18.16666666666667</v>
       </c>
       <c r="C6" t="n">
         <v>19</v>

</xml_diff>